<commit_message>
Published state of ETDataset on August 3 2021
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/biogas.carrier.xlsx
+++ b/carriers_source_analyses/biogas.carrier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/carriers_source_analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottevonm/Code/etdataset/carriers_source_analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934BD143-1DFA-0C47-8502-44B952D0A5E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C866D39-7FD4-7040-A60A-876AA8485A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2180" yWindow="500" windowWidth="25600" windowHeight="16060" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -42,6 +42,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -50,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="180">
   <si>
     <t>Source</t>
   </si>
@@ -176,12 +185,6 @@
   </si>
   <si>
     <t>Quintel assumption</t>
-  </si>
-  <si>
-    <t>Quintel definition</t>
-  </si>
-  <si>
-    <t>This is a definition</t>
   </si>
   <si>
     <t>kg/MJ</t>
@@ -624,7 +627,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;_-* #,##0.00\-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
@@ -633,7 +636,6 @@
     <numFmt numFmtId="169" formatCode="0.0000000000"/>
     <numFmt numFmtId="170" formatCode="0.0%"/>
     <numFmt numFmtId="171" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="0.00000000000000"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -1563,7 +1565,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1787,7 +1789,6 @@
     <xf numFmtId="1" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="172" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1798,6 +1799,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1825,13 +1833,6 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="335">
     <cellStyle name="Comma" xfId="320" builtinId="3"/>
@@ -2168,7 +2169,7 @@
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="321" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="321" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -3363,13 +3364,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="29" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="2.1640625" style="21" customWidth="1"/>
-    <col min="5" max="16384" width="10.6640625" style="21"/>
+    <col min="1" max="1" width="3.42578125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="21" customWidth="1"/>
+    <col min="5" max="16384" width="10.7109375" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="27" customFormat="1">
@@ -3392,10 +3393,10 @@
     <row r="4" spans="1:4">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3432,13 +3433,13 @@
         <v>14</v>
       </c>
       <c r="C9" s="76"/>
-      <c r="D9" s="153"/>
+      <c r="D9" s="152"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="7"/>
       <c r="B10" s="77"/>
       <c r="C10" s="78"/>
-      <c r="D10" s="154"/>
+      <c r="D10" s="153"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="7"/>
@@ -3448,7 +3449,7 @@
       <c r="C11" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="154"/>
+      <c r="D11" s="153"/>
     </row>
     <row r="12" spans="1:4" ht="17" thickBot="1">
       <c r="A12" s="7"/>
@@ -3456,7 +3457,7 @@
       <c r="C12" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="154"/>
+      <c r="D12" s="153"/>
     </row>
     <row r="13" spans="1:4" ht="17" thickBot="1">
       <c r="A13" s="7"/>
@@ -3464,7 +3465,7 @@
       <c r="C13" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="154"/>
+      <c r="D13" s="153"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="7"/>
@@ -3472,13 +3473,13 @@
       <c r="C14" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="154"/>
+      <c r="D14" s="153"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="7"/>
       <c r="B15" s="77"/>
       <c r="C15" s="78"/>
-      <c r="D15" s="154"/>
+      <c r="D15" s="153"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="7"/>
@@ -3488,7 +3489,7 @@
       <c r="C16" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="154"/>
+      <c r="D16" s="153"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7"/>
@@ -3496,7 +3497,7 @@
       <c r="C17" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="154"/>
+      <c r="D17" s="153"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="7"/>
@@ -3504,7 +3505,7 @@
       <c r="C18" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="154"/>
+      <c r="D18" s="153"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="7"/>
@@ -3512,7 +3513,7 @@
       <c r="C19" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="154"/>
+      <c r="D19" s="153"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="7"/>
@@ -3520,7 +3521,7 @@
       <c r="C20" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="154"/>
+      <c r="D20" s="153"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="7"/>
@@ -3528,7 +3529,7 @@
       <c r="C21" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="154"/>
+      <c r="D21" s="153"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="7"/>
@@ -3536,19 +3537,19 @@
       <c r="C22" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="154"/>
+      <c r="D22" s="153"/>
     </row>
     <row r="23" spans="1:4">
       <c r="B23" s="85"/>
       <c r="C23" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="154"/>
+      <c r="D23" s="153"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="B24" s="155"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="157"/>
+      <c r="B24" s="154"/>
+      <c r="C24" s="155"/>
+      <c r="D24" s="156"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3561,25 +3562,25 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B1:J14"/>
+  <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" style="35" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" style="35" customWidth="1"/>
     <col min="3" max="3" width="46" style="35" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="35" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="35" customWidth="1"/>
-    <col min="6" max="6" width="4.5" style="35" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="35" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="35" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="35" customWidth="1"/>
     <col min="7" max="7" width="45" style="35" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" style="35" customWidth="1"/>
-    <col min="9" max="9" width="51.5" style="35" customWidth="1"/>
-    <col min="10" max="10" width="5.5" style="35" customWidth="1"/>
-    <col min="11" max="16384" width="10.6640625" style="35"/>
+    <col min="8" max="8" width="5.140625" style="35" customWidth="1"/>
+    <col min="9" max="9" width="51.42578125" style="35" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="35" customWidth="1"/>
+    <col min="11" max="16384" width="10.7109375" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
@@ -3589,28 +3590,28 @@
       <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
-      <c r="B2" s="162" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164"/>
+      <c r="B2" s="168" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="169"/>
+      <c r="D2" s="169"/>
+      <c r="E2" s="170"/>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="165"/>
-      <c r="C3" s="166"/>
-      <c r="D3" s="166"/>
-      <c r="E3" s="167"/>
+      <c r="B3" s="171"/>
+      <c r="C3" s="172"/>
+      <c r="D3" s="172"/>
+      <c r="E3" s="173"/>
       <c r="F3" s="33"/>
       <c r="G3" s="33"/>
     </row>
     <row r="4" spans="2:10" ht="60" customHeight="1">
-      <c r="B4" s="168"/>
-      <c r="C4" s="169"/>
-      <c r="D4" s="169"/>
-      <c r="E4" s="170"/>
+      <c r="B4" s="174"/>
+      <c r="C4" s="175"/>
+      <c r="D4" s="175"/>
+      <c r="E4" s="176"/>
       <c r="F4" s="33"/>
       <c r="G4" s="33"/>
     </row>
@@ -3662,8 +3663,8 @@
     </row>
     <row r="9" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
       <c r="B9" s="23"/>
-      <c r="C9" s="152" t="s">
-        <v>178</v>
+      <c r="C9" s="151" t="s">
+        <v>176</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="18"/>
@@ -3698,75 +3699,33 @@
     <row r="11" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
       <c r="B11" s="23"/>
       <c r="C11" s="103" t="s">
-        <v>37</v>
+        <v>174</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="151">
-        <f>'Research data'!G7</f>
-        <v>1.679782273069216E-2</v>
+        <v>45</v>
+      </c>
+      <c r="E11" s="43">
+        <f>'Research data'!G8</f>
+        <v>27.500000000000004</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="103"/>
       <c r="H11" s="30"/>
       <c r="I11" s="118" t="s">
-        <v>45</v>
+        <v>171</v>
       </c>
       <c r="J11" s="42"/>
     </row>
-    <row r="12" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
-      <c r="B12" s="23"/>
-      <c r="C12" s="103" t="s">
-        <v>176</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="43">
-        <f>'Research data'!G8</f>
-        <v>27.500000000000004</v>
-      </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="118" t="s">
-        <v>173</v>
-      </c>
-      <c r="J12" s="42"/>
-    </row>
-    <row r="13" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
-      <c r="B13" s="23"/>
-      <c r="C13" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="105">
-        <f>'Research data'!G9</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="34"/>
-      <c r="G13" s="103" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="30"/>
-      <c r="I13" s="104" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="42"/>
-    </row>
-    <row r="14" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
+    <row r="12" spans="2:10" ht="20" customHeight="1" thickBot="1">
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3788,25 +3747,25 @@
       <selection activeCell="B10" sqref="B10:R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="3.5" style="65" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="65" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="65" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="65" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="65" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="65" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" style="65" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" style="66" customWidth="1"/>
+    <col min="1" max="2" width="3.42578125" style="65" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" style="65" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="65" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="65" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="65" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="65" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" style="65" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="66" customWidth="1"/>
     <col min="10" max="10" width="3" style="66" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="66" customWidth="1"/>
-    <col min="12" max="12" width="3.33203125" style="66" customWidth="1"/>
-    <col min="13" max="13" width="8.5" style="66" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" style="66" customWidth="1"/>
-    <col min="15" max="16" width="8.5" style="66" customWidth="1"/>
-    <col min="17" max="17" width="2.6640625" style="66" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="66" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" style="66" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" style="66" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" style="66" customWidth="1"/>
+    <col min="15" max="16" width="8.42578125" style="66" customWidth="1"/>
+    <col min="17" max="17" width="2.7109375" style="66" customWidth="1"/>
     <col min="18" max="18" width="60" style="65" customWidth="1"/>
-    <col min="19" max="16384" width="10.6640625" style="65"/>
+    <col min="19" max="16384" width="10.7109375" style="65"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="17" thickBot="1"/>
@@ -3844,22 +3803,22 @@
       </c>
       <c r="H3" s="96"/>
       <c r="I3" s="63" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J3" s="63"/>
       <c r="K3" s="63" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L3" s="63"/>
       <c r="M3" s="63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N3" s="63"/>
       <c r="O3" s="63" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="P3" s="63" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="Q3" s="63"/>
       <c r="R3" s="1" t="s">
@@ -3888,7 +3847,7 @@
     <row r="5" spans="1:18" ht="17" thickBot="1">
       <c r="B5" s="71"/>
       <c r="C5" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
@@ -3947,7 +3906,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G7" s="117">
         <f>K7</f>
@@ -3966,23 +3925,23 @@
       <c r="O7" s="16"/>
       <c r="P7" s="16"/>
       <c r="Q7" s="16"/>
-      <c r="R7" s="158" t="s">
-        <v>179</v>
+      <c r="R7" s="157" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:18" s="6" customFormat="1" ht="17" thickBot="1">
       <c r="B8" s="5"/>
       <c r="C8" s="107" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D8" s="107" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" s="107" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G8" s="43">
         <f>I8</f>
@@ -4002,7 +3961,7 @@
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="149" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="6" customFormat="1" ht="17" thickBot="1">
@@ -4017,7 +3976,7 @@
         <v>38</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G9" s="43">
         <v>0</v>
@@ -4035,24 +3994,24 @@
       <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:18" ht="17" thickBot="1">
-      <c r="A10" s="173"/>
-      <c r="B10" s="174"/>
-      <c r="C10" s="172"/>
-      <c r="D10" s="171"/>
-      <c r="E10" s="171"/>
-      <c r="F10" s="172"/>
-      <c r="G10" s="175"/>
-      <c r="H10" s="172"/>
-      <c r="I10" s="176"/>
-      <c r="J10" s="176"/>
-      <c r="K10" s="176"/>
-      <c r="L10" s="176"/>
-      <c r="M10" s="176"/>
-      <c r="N10" s="176"/>
-      <c r="O10" s="176"/>
-      <c r="P10" s="176"/>
-      <c r="Q10" s="176"/>
-      <c r="R10" s="177"/>
+      <c r="A10" s="163"/>
+      <c r="B10" s="164"/>
+      <c r="C10" s="162"/>
+      <c r="D10" s="161"/>
+      <c r="E10" s="161"/>
+      <c r="F10" s="162"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="162"/>
+      <c r="I10" s="166"/>
+      <c r="J10" s="166"/>
+      <c r="K10" s="166"/>
+      <c r="L10" s="166"/>
+      <c r="M10" s="166"/>
+      <c r="N10" s="166"/>
+      <c r="O10" s="166"/>
+      <c r="P10" s="166"/>
+      <c r="Q10" s="166"/>
+      <c r="R10" s="167"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4071,19 +4030,19 @@
       <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="33.140625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="45" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="45" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="45" customWidth="1"/>
-    <col min="4" max="4" width="3.1640625" style="45" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" style="45" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" style="45" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="45" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="45" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="45" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="45" customWidth="1"/>
     <col min="6" max="6" width="5" style="45" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" style="45" customWidth="1"/>
-    <col min="8" max="10" width="12.1640625" style="45" customWidth="1"/>
-    <col min="11" max="11" width="33.1640625" style="46" customWidth="1"/>
-    <col min="12" max="12" width="87.33203125" style="45" customWidth="1"/>
-    <col min="13" max="16384" width="33.1640625" style="45"/>
+    <col min="7" max="7" width="10.28515625" style="45" customWidth="1"/>
+    <col min="8" max="10" width="12.140625" style="45" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" style="46" customWidth="1"/>
+    <col min="12" max="12" width="87.28515625" style="45" customWidth="1"/>
+    <col min="13" max="16384" width="33.140625" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="17" thickBot="1"/>
@@ -4173,27 +4132,27 @@
     <row r="7" spans="2:12">
       <c r="B7" s="50"/>
       <c r="C7" s="119" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D7" s="58"/>
       <c r="E7" s="150" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F7" s="150" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G7" s="53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H7" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I7" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J7" s="54"/>
       <c r="K7" s="54" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="L7" s="115"/>
     </row>
@@ -4204,20 +4163,20 @@
       </c>
       <c r="D8" s="59"/>
       <c r="E8" s="109" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H8" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I8" s="54" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J8" s="54"/>
       <c r="K8" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L8" s="64"/>
     </row>
@@ -4241,7 +4200,7 @@
       </c>
       <c r="D10" s="62"/>
       <c r="E10" s="109" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F10" s="114"/>
       <c r="G10" s="60"/>
@@ -4249,7 +4208,7 @@
       <c r="I10" s="61"/>
       <c r="J10" s="61"/>
       <c r="K10" s="54" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L10" s="115"/>
     </row>
@@ -4269,12 +4228,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="98" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="98" customWidth="1"/>
     <col min="2" max="2" width="5" style="98" customWidth="1"/>
     <col min="3" max="5" width="7" style="98"/>
-    <col min="6" max="6" width="10.83203125" style="98" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="98" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="98"/>
-    <col min="8" max="8" width="8.83203125" style="98" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="98" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="7" style="98"/>
   </cols>
   <sheetData>
@@ -4285,7 +4244,7 @@
         <v>24</v>
       </c>
       <c r="D2" s="102" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E2" s="102"/>
       <c r="F2" s="102" t="s">
@@ -4357,7 +4316,7 @@
     <row r="5" spans="2:26" customFormat="1">
       <c r="B5" s="99"/>
       <c r="C5" s="109" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" s="109"/>
       <c r="E5" s="109"/>
@@ -4414,11 +4373,11 @@
       <c r="B7" s="99"/>
       <c r="C7" s="109"/>
       <c r="D7" s="109" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" s="109"/>
       <c r="F7" s="109" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G7" s="109"/>
       <c r="H7" s="109"/>
@@ -4447,7 +4406,7 @@
       <c r="D8" s="109"/>
       <c r="E8" s="109"/>
       <c r="F8" s="109" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G8" s="109"/>
       <c r="H8" s="109"/>
@@ -4825,7 +4784,7 @@
       <c r="B22" s="99"/>
       <c r="C22" s="109"/>
       <c r="D22" s="109" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E22" s="109"/>
       <c r="F22" s="109"/>
@@ -4856,7 +4815,7 @@
       <c r="D23" s="109"/>
       <c r="E23" s="109"/>
       <c r="F23" s="109" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G23" s="109"/>
       <c r="H23" s="120">
@@ -4887,7 +4846,7 @@
       <c r="D24" s="109"/>
       <c r="E24" s="109"/>
       <c r="F24" s="109" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G24" s="109"/>
       <c r="H24" s="121">
@@ -4918,14 +4877,14 @@
       <c r="D25" s="109"/>
       <c r="E25" s="109"/>
       <c r="F25" s="109" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G25" s="109"/>
       <c r="H25" s="109">
         <v>47.4</v>
       </c>
       <c r="I25" s="109" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J25" s="109"/>
       <c r="K25" s="109"/>
@@ -4951,14 +4910,14 @@
       <c r="D26" s="109"/>
       <c r="E26" s="109"/>
       <c r="F26" s="109" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G26" s="109"/>
       <c r="H26" s="109">
         <v>14.2</v>
       </c>
       <c r="I26" s="109" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J26" s="109"/>
       <c r="K26" s="109"/>
@@ -4984,7 +4943,7 @@
       <c r="D27" s="109"/>
       <c r="E27" s="109"/>
       <c r="F27" s="109" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G27" s="109"/>
       <c r="H27" s="122">
@@ -4992,7 +4951,7 @@
         <v>13.632</v>
       </c>
       <c r="I27" s="109" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J27" s="109"/>
       <c r="K27" s="109"/>
@@ -5018,7 +4977,7 @@
       <c r="D28" s="109"/>
       <c r="E28" s="109"/>
       <c r="F28" s="145" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G28" s="145"/>
       <c r="H28" s="147">
@@ -5026,7 +4985,7 @@
         <v>1363.2</v>
       </c>
       <c r="I28" s="145" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J28" s="109"/>
       <c r="K28" s="109"/>
@@ -5052,14 +5011,14 @@
       <c r="D29" s="109"/>
       <c r="E29" s="109"/>
       <c r="F29" s="109" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G29" s="109"/>
       <c r="H29" s="109">
         <v>575</v>
       </c>
       <c r="I29" s="123" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J29" s="109"/>
       <c r="K29" s="109"/>
@@ -5085,7 +5044,7 @@
       <c r="D30" s="109"/>
       <c r="E30" s="109"/>
       <c r="F30" s="109" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G30" s="109"/>
       <c r="H30" s="121">
@@ -5116,7 +5075,7 @@
       <c r="D31" s="109"/>
       <c r="E31" s="109"/>
       <c r="F31" s="109" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G31" s="109"/>
       <c r="H31" s="109">
@@ -5124,7 +5083,7 @@
         <v>316.25</v>
       </c>
       <c r="I31" s="123" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J31" s="109"/>
       <c r="K31" s="109"/>
@@ -5150,14 +5109,14 @@
       <c r="D32" s="109"/>
       <c r="E32" s="109"/>
       <c r="F32" s="124" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G32" s="124"/>
       <c r="H32" s="109">
         <v>55.5</v>
       </c>
       <c r="I32" s="123" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J32" s="109"/>
       <c r="K32" s="109"/>
@@ -5183,7 +5142,7 @@
       <c r="D33" s="109"/>
       <c r="E33" s="109"/>
       <c r="F33" s="124" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G33" s="124"/>
       <c r="H33" s="109">
@@ -5191,7 +5150,7 @@
         <v>50</v>
       </c>
       <c r="I33" s="123" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J33" s="109"/>
       <c r="K33" s="109"/>
@@ -5217,14 +5176,14 @@
       <c r="D34" s="109"/>
       <c r="E34" s="109"/>
       <c r="F34" s="124" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G34" s="124"/>
       <c r="H34" s="109">
         <v>7.1599999999999995E-4</v>
       </c>
       <c r="I34" s="123" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J34" s="109"/>
       <c r="K34" s="109"/>
@@ -5250,7 +5209,7 @@
       <c r="D35" s="109"/>
       <c r="E35" s="109"/>
       <c r="F35" s="124" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G35" s="124"/>
       <c r="H35" s="109">
@@ -5258,7 +5217,7 @@
         <v>39.737999999999992</v>
       </c>
       <c r="I35" s="123" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J35" s="109"/>
       <c r="K35" s="109"/>
@@ -5284,7 +5243,7 @@
       <c r="D36" s="109"/>
       <c r="E36" s="109"/>
       <c r="F36" s="124" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G36" s="124"/>
       <c r="H36" s="109">
@@ -5292,7 +5251,7 @@
         <v>35.799999999999997</v>
       </c>
       <c r="I36" s="123" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J36" s="109"/>
       <c r="K36" s="109"/>
@@ -5318,7 +5277,7 @@
       <c r="D37" s="109"/>
       <c r="E37" s="109"/>
       <c r="F37" s="109" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G37" s="109"/>
       <c r="H37" s="109">
@@ -5326,7 +5285,7 @@
         <v>11.32175</v>
       </c>
       <c r="I37" s="123" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J37" s="109"/>
       <c r="K37" s="109"/>
@@ -5352,7 +5311,7 @@
       <c r="D38" s="109"/>
       <c r="E38" s="109"/>
       <c r="F38" s="109" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G38" s="109"/>
       <c r="H38" s="109">
@@ -5360,7 +5319,7 @@
         <v>11.32175</v>
       </c>
       <c r="I38" s="123" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J38" s="109"/>
       <c r="K38" s="109"/>
@@ -5386,7 +5345,7 @@
       <c r="D39" s="109"/>
       <c r="E39" s="109"/>
       <c r="F39" s="145" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G39" s="146"/>
       <c r="H39" s="148">
@@ -5394,7 +5353,7 @@
         <v>15433809.6</v>
       </c>
       <c r="I39" s="123" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J39" s="109"/>
       <c r="K39" s="109"/>
@@ -6154,7 +6113,7 @@
       <c r="B67" s="99"/>
       <c r="C67" s="109"/>
       <c r="D67" s="109" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E67" s="109"/>
       <c r="F67" s="109"/>
@@ -6185,14 +6144,14 @@
       <c r="D68" s="125"/>
       <c r="E68" s="125"/>
       <c r="F68" s="125" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G68" s="125"/>
       <c r="H68" s="126">
         <v>0.90800000000000003</v>
       </c>
       <c r="I68" s="127" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K68" s="125"/>
       <c r="L68" s="125"/>
@@ -6217,14 +6176,14 @@
       <c r="D69" s="125"/>
       <c r="E69" s="125"/>
       <c r="F69" s="129" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G69" s="129"/>
       <c r="H69" s="126">
         <v>7.8E-2</v>
       </c>
       <c r="I69" s="127" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K69" s="125"/>
       <c r="L69" s="125"/>
@@ -6249,14 +6208,14 @@
       <c r="D70" s="125"/>
       <c r="E70" s="125"/>
       <c r="F70" s="129" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G70" s="129"/>
       <c r="H70" s="126">
         <v>1.4E-2</v>
       </c>
       <c r="I70" s="127" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K70" s="125"/>
       <c r="L70" s="125"/>
@@ -6281,17 +6240,17 @@
       <c r="D71" s="125"/>
       <c r="E71" s="125"/>
       <c r="F71" s="130" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G71" s="130"/>
       <c r="H71" s="131">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="I71" s="132" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K71" s="125" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L71" s="125"/>
       <c r="M71" s="125"/>
@@ -6341,14 +6300,14 @@
       <c r="D73" s="125"/>
       <c r="E73" s="125"/>
       <c r="F73" s="125" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G73" s="125"/>
       <c r="H73" s="126">
         <v>0.99099999999999999</v>
       </c>
       <c r="I73" s="127" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K73" s="125"/>
       <c r="L73" s="125"/>
@@ -6373,14 +6332,14 @@
       <c r="D74" s="125"/>
       <c r="E74" s="125"/>
       <c r="F74" s="129" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G74" s="129"/>
       <c r="H74" s="133">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="I74" s="127" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K74" s="125"/>
       <c r="L74" s="125"/>
@@ -6431,17 +6390,17 @@
       <c r="D76" s="109"/>
       <c r="E76" s="109"/>
       <c r="F76" s="130" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G76" s="130"/>
       <c r="H76" s="135">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="I76" s="132" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K76" s="125" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L76" s="109"/>
       <c r="M76" s="109"/>
@@ -6465,17 +6424,17 @@
       <c r="D77" s="109"/>
       <c r="E77" s="109"/>
       <c r="F77" s="130" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G77" s="130"/>
       <c r="H77" s="136">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="I77" s="132" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K77" s="125" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L77" s="109"/>
       <c r="M77" s="109"/>
@@ -7874,7 +7833,7 @@
       <c r="B129" s="99"/>
       <c r="C129" s="109"/>
       <c r="D129" s="109" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E129" s="109"/>
       <c r="F129" s="109"/>
@@ -7905,14 +7864,14 @@
       <c r="D130" s="109"/>
       <c r="E130" s="109"/>
       <c r="F130" s="112" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G130" s="112"/>
       <c r="H130" s="112" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I130" s="112" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J130" s="109"/>
       <c r="K130" s="109"/>
@@ -7938,7 +7897,7 @@
       <c r="D131" s="109"/>
       <c r="E131" s="109"/>
       <c r="F131" s="112" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G131" s="112"/>
       <c r="H131" s="112"/>
@@ -7967,14 +7926,14 @@
       <c r="D132" s="109"/>
       <c r="E132" s="109"/>
       <c r="F132" s="137" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G132" s="137"/>
       <c r="H132" s="138">
         <v>1248457</v>
       </c>
       <c r="I132" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J132" s="109"/>
       <c r="K132" s="138"/>
@@ -8000,14 +7959,14 @@
       <c r="D133" s="109"/>
       <c r="E133" s="109"/>
       <c r="F133" s="137" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G133" s="137"/>
       <c r="H133" s="138">
         <v>1564661</v>
       </c>
       <c r="I133" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J133" s="109"/>
       <c r="K133" s="138"/>
@@ -8033,14 +7992,14 @@
       <c r="D134" s="109"/>
       <c r="E134" s="109"/>
       <c r="F134" s="109" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G134" s="109"/>
       <c r="H134" s="138">
         <v>79384</v>
       </c>
       <c r="I134" s="109" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J134" s="109"/>
       <c r="K134" s="138"/>
@@ -8066,7 +8025,7 @@
       <c r="D135" s="109"/>
       <c r="E135" s="109"/>
       <c r="F135" s="109" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G135" s="109"/>
       <c r="H135" s="139">
@@ -8074,12 +8033,12 @@
         <v>17.718419328832006</v>
       </c>
       <c r="I135" s="109" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J135" s="109"/>
       <c r="K135" s="139"/>
       <c r="L135" s="112" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M135" s="109"/>
       <c r="N135" s="109"/>
@@ -8129,7 +8088,7 @@
       <c r="D137" s="109"/>
       <c r="E137" s="109"/>
       <c r="F137" s="112" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G137" s="112"/>
       <c r="H137" s="112"/>
@@ -8158,14 +8117,14 @@
       <c r="D138" s="109"/>
       <c r="E138" s="109"/>
       <c r="F138" s="137" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G138" s="137"/>
       <c r="H138" s="138">
         <v>1468130</v>
       </c>
       <c r="I138" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J138" s="109"/>
       <c r="K138" s="139"/>
@@ -8191,14 +8150,14 @@
       <c r="D139" s="109"/>
       <c r="E139" s="109"/>
       <c r="F139" s="137" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G139" s="137"/>
       <c r="H139" s="138">
         <v>1777989</v>
       </c>
       <c r="I139" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J139" s="109"/>
       <c r="K139" s="139"/>
@@ -8224,14 +8183,14 @@
       <c r="D140" s="109"/>
       <c r="E140" s="109"/>
       <c r="F140" s="109" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G140" s="109"/>
       <c r="H140" s="138">
         <v>79384</v>
       </c>
       <c r="I140" s="109" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J140" s="109"/>
       <c r="K140" s="139"/>
@@ -8257,7 +8216,7 @@
       <c r="D141" s="109"/>
       <c r="E141" s="109"/>
       <c r="F141" s="109" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G141" s="109"/>
       <c r="H141" s="138">
@@ -8265,7 +8224,7 @@
         <v>78669.543999999994</v>
       </c>
       <c r="I141" s="109" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J141" s="109"/>
       <c r="K141" s="139"/>
@@ -8291,7 +8250,7 @@
       <c r="D142" s="109"/>
       <c r="E142" s="109"/>
       <c r="F142" s="109" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G142" s="109"/>
       <c r="H142" s="139">
@@ -8299,7 +8258,7 @@
         <v>20.631357670002512</v>
       </c>
       <c r="I142" s="109" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J142" s="109"/>
       <c r="K142" s="139"/>
@@ -8352,7 +8311,7 @@
       <c r="D144" s="109"/>
       <c r="E144" s="109"/>
       <c r="F144" s="109" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G144" s="109"/>
       <c r="H144" s="109"/>
@@ -8381,14 +8340,14 @@
       <c r="D145" s="109"/>
       <c r="E145" s="109"/>
       <c r="F145" s="112" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G145" s="112"/>
       <c r="H145" s="112">
         <v>2000</v>
       </c>
       <c r="I145" s="112" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J145" s="109"/>
       <c r="K145" s="109"/>
@@ -8414,7 +8373,7 @@
       <c r="D146" s="109"/>
       <c r="E146" s="109"/>
       <c r="F146" s="112" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G146" s="112"/>
       <c r="H146" s="112"/>
@@ -8443,14 +8402,14 @@
       <c r="D147" s="109"/>
       <c r="E147" s="109"/>
       <c r="F147" s="137" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G147" s="137"/>
       <c r="H147" s="138">
         <v>4520492</v>
       </c>
       <c r="I147" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J147" s="138"/>
       <c r="K147" s="109"/>
@@ -8476,14 +8435,14 @@
       <c r="D148" s="109"/>
       <c r="E148" s="109"/>
       <c r="F148" s="137" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G148" s="137"/>
       <c r="H148" s="138">
         <v>5562658</v>
       </c>
       <c r="I148" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J148" s="138"/>
       <c r="K148" s="109"/>
@@ -8509,14 +8468,14 @@
       <c r="D149" s="109"/>
       <c r="E149" s="109"/>
       <c r="F149" s="109" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G149" s="109"/>
       <c r="H149" s="138">
         <v>317535</v>
       </c>
       <c r="I149" s="109" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J149" s="109"/>
       <c r="K149" s="109"/>
@@ -8542,7 +8501,7 @@
       <c r="D150" s="109"/>
       <c r="E150" s="109"/>
       <c r="F150" s="109" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G150" s="109"/>
       <c r="H150" s="139">
@@ -8550,7 +8509,7 @@
         <v>15.877226132552318</v>
       </c>
       <c r="I150" s="109" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J150" s="109"/>
       <c r="K150" s="109"/>
@@ -8603,7 +8562,7 @@
       <c r="D152" s="109"/>
       <c r="E152" s="109"/>
       <c r="F152" s="112" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G152" s="112"/>
       <c r="H152" s="112"/>
@@ -8632,14 +8591,14 @@
       <c r="D153" s="109"/>
       <c r="E153" s="109"/>
       <c r="F153" s="137" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G153" s="137"/>
       <c r="H153" s="138">
         <v>5069011</v>
       </c>
       <c r="I153" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J153" s="109"/>
       <c r="K153" s="109"/>
@@ -8665,14 +8624,14 @@
       <c r="D154" s="109"/>
       <c r="E154" s="109"/>
       <c r="F154" s="137" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G154" s="137"/>
       <c r="H154" s="138">
         <v>6103024</v>
       </c>
       <c r="I154" s="109" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J154" s="109"/>
       <c r="K154" s="109"/>
@@ -8698,14 +8657,14 @@
       <c r="D155" s="109"/>
       <c r="E155" s="109"/>
       <c r="F155" s="109" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G155" s="109"/>
       <c r="H155" s="138">
         <v>317535</v>
       </c>
       <c r="I155" s="109" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J155" s="109"/>
       <c r="K155" s="109"/>
@@ -8731,7 +8690,7 @@
       <c r="D156" s="109"/>
       <c r="E156" s="109"/>
       <c r="F156" s="109" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G156" s="109"/>
       <c r="H156" s="138">
@@ -8739,7 +8698,7 @@
         <v>314677.185</v>
       </c>
       <c r="I156" s="109" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J156" s="109"/>
       <c r="K156" s="109"/>
@@ -8765,7 +8724,7 @@
       <c r="D157" s="109"/>
       <c r="E157" s="109"/>
       <c r="F157" s="109" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G157" s="109"/>
       <c r="H157" s="139">
@@ -8773,7 +8732,7 @@
         <v>17.751580878035373</v>
       </c>
       <c r="I157" s="109" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J157" s="109"/>
       <c r="K157" s="109"/>
@@ -9852,7 +9811,7 @@
       <c r="D197" s="109"/>
       <c r="E197" s="109"/>
       <c r="F197" s="109" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G197" s="109"/>
       <c r="H197" s="109"/>
@@ -9908,7 +9867,7 @@
       <c r="D199" s="109"/>
       <c r="E199" s="109"/>
       <c r="F199" s="109" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G199" s="109"/>
       <c r="H199" s="109"/>
@@ -9968,7 +9927,7 @@
         <v>64.79281693354568</v>
       </c>
       <c r="I201" s="109" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K201" s="109"/>
       <c r="L201" s="109"/>
@@ -9997,7 +9956,7 @@
         <v>7716.9048000000012</v>
       </c>
       <c r="I202" s="109" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K202" s="109"/>
       <c r="L202" s="109"/>
@@ -10025,7 +9984,7 @@
         <v>1000000</v>
       </c>
       <c r="I203" s="109" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J203" s="109"/>
       <c r="K203" s="109"/>
@@ -10055,7 +10014,7 @@
         <v>500000</v>
       </c>
       <c r="I204" s="109" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J204" s="109"/>
       <c r="K204" s="109"/>
@@ -10189,7 +10148,7 @@
       <c r="D209" s="109"/>
       <c r="E209" s="109"/>
       <c r="F209" s="109" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G209" s="109"/>
       <c r="H209" s="109"/>
@@ -10216,18 +10175,18 @@
       <c r="B210" s="99"/>
       <c r="C210" s="109"/>
       <c r="D210" s="109" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E210" s="109"/>
       <c r="F210" s="123" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G210" s="123"/>
       <c r="H210" s="109">
         <v>21</v>
       </c>
       <c r="I210" s="109" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K210" s="109"/>
       <c r="L210" s="109"/>
@@ -10279,7 +10238,7 @@
       <c r="D212" s="109"/>
       <c r="E212" s="109"/>
       <c r="F212" s="109" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G212" s="109"/>
       <c r="H212" s="144">
@@ -10287,7 +10246,7 @@
         <v>1420</v>
       </c>
       <c r="I212" s="123" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K212" s="109"/>
       <c r="M212" s="109"/>
@@ -10311,7 +10270,7 @@
       <c r="D213" s="109"/>
       <c r="E213" s="109"/>
       <c r="F213" s="109" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G213" s="109"/>
       <c r="H213" s="144">
@@ -10319,7 +10278,7 @@
         <v>7716.9048000000012</v>
       </c>
       <c r="I213" s="123" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K213" s="109"/>
       <c r="M213" s="109"/>
@@ -10343,7 +10302,7 @@
       <c r="D214" s="109"/>
       <c r="E214" s="109"/>
       <c r="F214" s="109" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G214" s="109"/>
       <c r="H214" s="144">
@@ -10351,10 +10310,10 @@
         <v>5.4344400000000004</v>
       </c>
       <c r="I214" s="123" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J214" s="109" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K214" s="109"/>
       <c r="M214" s="109"/>
@@ -10378,7 +10337,7 @@
       <c r="D215" s="109"/>
       <c r="E215" s="109"/>
       <c r="F215" s="109" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G215" s="109"/>
       <c r="H215" s="140">
@@ -10386,7 +10345,7 @@
         <v>3.8642436019166646</v>
       </c>
       <c r="I215" s="123" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K215" s="109"/>
       <c r="M215" s="109"/>
@@ -10488,7 +10447,7 @@
         <v>24</v>
       </c>
       <c r="D219" s="102" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E219" s="102"/>
       <c r="F219" s="102" t="s">
@@ -10564,7 +10523,7 @@
     <row r="222" spans="2:26" customFormat="1">
       <c r="B222" s="99"/>
       <c r="C222" s="109" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D222" s="109"/>
       <c r="E222" s="109"/>
@@ -10618,7 +10577,7 @@
       <c r="B224" s="99"/>
       <c r="C224" s="109"/>
       <c r="D224" s="109" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E224" s="109"/>
       <c r="F224" s="109"/>
@@ -10648,14 +10607,14 @@
       <c r="D225" s="109"/>
       <c r="E225" s="109"/>
       <c r="F225" s="109" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G225" s="109"/>
       <c r="H225" s="109">
         <v>47.4</v>
       </c>
       <c r="I225" s="109" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J225" s="109"/>
       <c r="K225" s="109"/>
@@ -10681,14 +10640,14 @@
       <c r="D226" s="109"/>
       <c r="E226" s="109"/>
       <c r="F226" s="109" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G226" s="109"/>
       <c r="H226" s="109">
         <v>14.2</v>
       </c>
       <c r="I226" s="109" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J226" s="109"/>
       <c r="K226" s="109"/>
@@ -11604,7 +11563,7 @@
         <v>24</v>
       </c>
       <c r="D260" s="102" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E260" s="102"/>
       <c r="F260" s="102" t="s">
@@ -11655,12 +11614,12 @@
     <row r="262" spans="2:26" customFormat="1">
       <c r="B262" s="99"/>
       <c r="C262" s="109" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D262" s="109"/>
       <c r="E262" s="109"/>
       <c r="F262" s="109" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G262" s="109"/>
       <c r="H262" s="109"/>
@@ -11700,11 +11659,11 @@
       <c r="B264" s="99"/>
       <c r="C264" s="109"/>
       <c r="D264" s="109" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E264" s="109"/>
       <c r="F264" s="109" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G264" s="109"/>
       <c r="H264" s="109"/>
@@ -11813,7 +11772,7 @@
       <c r="D269" s="109"/>
       <c r="E269" s="109"/>
       <c r="F269" s="112" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G269" s="112"/>
       <c r="H269" s="109"/>
@@ -11837,12 +11796,12 @@
       <c r="D270" s="109"/>
       <c r="E270" s="109"/>
       <c r="F270" s="109" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G270" s="109"/>
       <c r="H270" s="109"/>
       <c r="I270" s="109" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J270" s="109"/>
       <c r="K270" s="109"/>
@@ -11863,14 +11822,14 @@
       <c r="D271" s="109"/>
       <c r="E271" s="109"/>
       <c r="F271" s="109" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G271" s="109"/>
       <c r="H271" s="109">
         <v>16.7</v>
       </c>
       <c r="I271" s="109" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J271" s="109"/>
       <c r="K271" s="109"/>
@@ -11891,14 +11850,14 @@
       <c r="D272" s="109"/>
       <c r="E272" s="109"/>
       <c r="F272" s="109" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G272" s="109"/>
       <c r="H272" s="109">
         <v>61.145000000000003</v>
       </c>
       <c r="I272" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J272" s="109"/>
       <c r="K272" s="109"/>
@@ -11919,14 +11878,14 @@
       <c r="D273" s="109"/>
       <c r="E273" s="109"/>
       <c r="F273" s="109" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G273" s="109"/>
       <c r="H273" s="109">
         <v>4.8920000000000003</v>
       </c>
       <c r="I273" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J273" s="109"/>
       <c r="K273" s="109"/>
@@ -11947,7 +11906,7 @@
       <c r="D274" s="109"/>
       <c r="E274" s="109"/>
       <c r="F274" s="109" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G274" s="109"/>
       <c r="H274" s="122">
@@ -11974,14 +11933,14 @@
       <c r="D275" s="109"/>
       <c r="E275" s="109"/>
       <c r="F275" s="109" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G275" s="109"/>
       <c r="H275" s="109">
         <v>12.228999999999999</v>
       </c>
       <c r="I275" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J275" s="109"/>
       <c r="K275" s="109"/>
@@ -12002,14 +11961,14 @@
       <c r="D276" s="109"/>
       <c r="E276" s="109"/>
       <c r="F276" s="109" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G276" s="109"/>
       <c r="H276" s="109">
         <v>0.97799999999999998</v>
       </c>
       <c r="I276" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J276" s="109"/>
       <c r="K276" s="109"/>
@@ -12084,7 +12043,7 @@
       <c r="D280" s="109"/>
       <c r="E280" s="109"/>
       <c r="F280" s="112" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G280" s="112"/>
       <c r="H280" s="109"/>
@@ -12108,14 +12067,14 @@
       <c r="D281" s="109"/>
       <c r="E281" s="109"/>
       <c r="F281" s="109" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G281" s="109"/>
       <c r="H281" s="109">
         <v>6.6</v>
       </c>
       <c r="I281" s="109" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J281" s="109"/>
       <c r="K281" s="109"/>
@@ -12136,14 +12095,14 @@
       <c r="D282" s="109"/>
       <c r="E282" s="109"/>
       <c r="F282" s="109" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G282" s="109"/>
       <c r="H282" s="109">
         <v>16</v>
       </c>
       <c r="I282" s="109" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J282" s="109"/>
       <c r="K282" s="109"/>
@@ -12164,14 +12123,14 @@
       <c r="D283" s="109"/>
       <c r="E283" s="109"/>
       <c r="F283" s="109" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G283" s="109"/>
       <c r="H283" s="109">
         <v>5.4039999999999999</v>
       </c>
       <c r="I283" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J283" s="109"/>
       <c r="K283" s="109"/>
@@ -12192,14 +12151,14 @@
       <c r="D284" s="109"/>
       <c r="E284" s="109"/>
       <c r="F284" s="109" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G284" s="109"/>
       <c r="H284" s="109">
         <v>2.972</v>
       </c>
       <c r="I284" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J284" s="109"/>
       <c r="K284" s="109"/>
@@ -12220,7 +12179,7 @@
       <c r="D285" s="109"/>
       <c r="E285" s="109"/>
       <c r="F285" s="109" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G285" s="109"/>
       <c r="H285" s="122">
@@ -12247,14 +12206,14 @@
       <c r="D286" s="109"/>
       <c r="E286" s="109"/>
       <c r="F286" s="109" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G286" s="109"/>
       <c r="H286" s="109">
         <v>2.7280000000000002</v>
       </c>
       <c r="I286" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J286" s="109"/>
       <c r="K286" s="109"/>
@@ -12275,14 +12234,14 @@
       <c r="D287" s="109"/>
       <c r="E287" s="109"/>
       <c r="F287" s="109" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G287" s="109"/>
       <c r="H287" s="109">
         <v>1.5009999999999999</v>
       </c>
       <c r="I287" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J287" s="109"/>
       <c r="K287" s="109"/>
@@ -12325,7 +12284,7 @@
       <c r="D289" s="109"/>
       <c r="E289" s="109"/>
       <c r="F289" s="112" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G289" s="112"/>
       <c r="H289" s="109"/>
@@ -12349,7 +12308,7 @@
       <c r="D290" s="109"/>
       <c r="E290" s="109"/>
       <c r="F290" s="109" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G290" s="109"/>
       <c r="H290" s="109">
@@ -12357,7 +12316,7 @@
         <v>16.350000000000001</v>
       </c>
       <c r="I290" s="109" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J290" s="109"/>
       <c r="K290" s="109"/>
@@ -12400,7 +12359,7 @@
       <c r="D292" s="109"/>
       <c r="E292" s="109"/>
       <c r="F292" s="112" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G292" s="112"/>
       <c r="H292" s="109"/>
@@ -12424,7 +12383,7 @@
       <c r="D293" s="109"/>
       <c r="E293" s="109"/>
       <c r="F293" s="109" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G293" s="109"/>
       <c r="H293" s="109">
@@ -12432,7 +12391,7 @@
         <v>2.4790000000000001</v>
       </c>
       <c r="I293" s="109" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J293" s="109"/>
       <c r="K293" s="109"/>
@@ -12453,7 +12412,7 @@
       <c r="D294" s="109"/>
       <c r="E294" s="109"/>
       <c r="F294" s="109" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G294" s="109"/>
       <c r="H294" s="122">
@@ -12461,7 +12420,7 @@
         <v>40.348599999999998</v>
       </c>
       <c r="I294" s="109" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J294" s="109"/>
       <c r="K294" s="109"/>
@@ -12658,7 +12617,7 @@
         <v>24</v>
       </c>
       <c r="D303" s="102" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E303" s="102"/>
       <c r="F303" s="102" t="s">
@@ -12709,7 +12668,7 @@
     <row r="305" spans="2:21" customFormat="1">
       <c r="B305" s="99"/>
       <c r="C305" s="115" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D305" s="109"/>
       <c r="E305" s="109"/>
@@ -12757,14 +12716,14 @@
       <c r="D307" s="109"/>
       <c r="E307" s="109"/>
       <c r="F307" s="109" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G307" s="109"/>
       <c r="H307" s="109">
         <v>72703</v>
       </c>
       <c r="I307" s="109" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J307" s="109"/>
       <c r="K307" s="109"/>
@@ -12785,7 +12744,7 @@
       <c r="D308" s="109"/>
       <c r="E308" s="109"/>
       <c r="F308" s="109" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G308" s="109"/>
       <c r="H308" s="109">
@@ -12793,7 +12752,7 @@
         <v>72.703000000000003</v>
       </c>
       <c r="I308" s="109" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J308" s="109"/>
       <c r="K308" s="109"/>
@@ -13474,7 +13433,7 @@
         <v>24</v>
       </c>
       <c r="D339" s="102" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E339" s="102"/>
       <c r="F339" s="102" t="s">
@@ -13525,7 +13484,7 @@
     <row r="341" spans="2:25" customFormat="1">
       <c r="B341" s="99"/>
       <c r="C341" s="109" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D341" s="109"/>
       <c r="E341" s="109"/>
@@ -13636,10 +13595,10 @@
       </c>
       <c r="F345" s="109"/>
       <c r="G345" s="110" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H345" s="111" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I345" s="109"/>
       <c r="J345" s="109"/>
@@ -13667,10 +13626,10 @@
         <v>50</v>
       </c>
       <c r="G346" s="109" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H346" s="111" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I346" s="109"/>
       <c r="J346" s="109"/>
@@ -13696,10 +13655,10 @@
       <c r="D347" s="109"/>
       <c r="F347" s="109"/>
       <c r="G347" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H347" s="111" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I347" s="109"/>
       <c r="J347" s="109"/>
@@ -13725,10 +13684,10 @@
       <c r="D348" s="109"/>
       <c r="F348" s="109"/>
       <c r="G348" s="109" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H348" s="111" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I348" s="109"/>
       <c r="J348" s="109"/>
@@ -13784,7 +13743,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="G350" s="109" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H350" s="109"/>
       <c r="I350" s="109"/>
@@ -13810,17 +13769,17 @@
       <c r="C351" s="109"/>
       <c r="D351" s="109"/>
       <c r="E351" s="109" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F351" s="109">
         <f>F350*F346</f>
         <v>27.500000000000004</v>
       </c>
       <c r="G351" s="109" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H351" s="109" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I351" s="109"/>
       <c r="J351" s="109"/>
@@ -14309,7 +14268,7 @@
         <v>24</v>
       </c>
       <c r="D399" s="102" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E399" s="102"/>
       <c r="F399" s="102" t="s">
@@ -14360,7 +14319,7 @@
     <row r="401" spans="2:25" customFormat="1">
       <c r="B401" s="99"/>
       <c r="C401" s="114" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D401" s="109"/>
       <c r="E401" s="109"/>
@@ -15285,19 +15244,19 @@
     <row r="514" spans="2:7" customFormat="1">
       <c r="B514" s="99"/>
       <c r="G514" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="515" spans="2:7" customFormat="1">
       <c r="B515" s="99"/>
       <c r="G515" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="516" spans="2:7" customFormat="1">
       <c r="B516" s="99"/>
       <c r="G516" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="517" spans="2:7" customFormat="1">
@@ -15351,41 +15310,41 @@
     <row r="533" spans="2:35" customFormat="1">
       <c r="B533" s="99"/>
     </row>
-    <row r="534" spans="2:35" s="159" customFormat="1">
-      <c r="B534" s="160"/>
-      <c r="C534" s="161"/>
-      <c r="D534" s="161"/>
-      <c r="E534" s="161"/>
-      <c r="F534" s="161"/>
-      <c r="G534" s="161"/>
-      <c r="H534" s="161"/>
-      <c r="I534" s="161"/>
-      <c r="J534" s="161"/>
-      <c r="K534" s="161"/>
-      <c r="L534" s="161"/>
-      <c r="M534" s="161"/>
-      <c r="N534" s="161"/>
-      <c r="O534" s="161"/>
-      <c r="P534" s="161"/>
-      <c r="Q534" s="161"/>
-      <c r="R534" s="161"/>
-      <c r="S534" s="161"/>
-      <c r="T534" s="161"/>
-      <c r="U534" s="161"/>
-      <c r="V534" s="161"/>
-      <c r="W534" s="161"/>
-      <c r="X534" s="161"/>
-      <c r="Y534" s="161"/>
-      <c r="Z534" s="161"/>
-      <c r="AA534" s="161"/>
-      <c r="AB534" s="161"/>
-      <c r="AC534" s="161"/>
-      <c r="AD534" s="161"/>
-      <c r="AE534" s="161"/>
-      <c r="AF534" s="161"/>
-      <c r="AG534" s="161"/>
-      <c r="AH534" s="161"/>
-      <c r="AI534" s="161"/>
+    <row r="534" spans="2:35" s="158" customFormat="1">
+      <c r="B534" s="159"/>
+      <c r="C534" s="160"/>
+      <c r="D534" s="160"/>
+      <c r="E534" s="160"/>
+      <c r="F534" s="160"/>
+      <c r="G534" s="160"/>
+      <c r="H534" s="160"/>
+      <c r="I534" s="160"/>
+      <c r="J534" s="160"/>
+      <c r="K534" s="160"/>
+      <c r="L534" s="160"/>
+      <c r="M534" s="160"/>
+      <c r="N534" s="160"/>
+      <c r="O534" s="160"/>
+      <c r="P534" s="160"/>
+      <c r="Q534" s="160"/>
+      <c r="R534" s="160"/>
+      <c r="S534" s="160"/>
+      <c r="T534" s="160"/>
+      <c r="U534" s="160"/>
+      <c r="V534" s="160"/>
+      <c r="W534" s="160"/>
+      <c r="X534" s="160"/>
+      <c r="Y534" s="160"/>
+      <c r="Z534" s="160"/>
+      <c r="AA534" s="160"/>
+      <c r="AB534" s="160"/>
+      <c r="AC534" s="160"/>
+      <c r="AD534" s="160"/>
+      <c r="AE534" s="160"/>
+      <c r="AF534" s="160"/>
+      <c r="AG534" s="160"/>
+      <c r="AH534" s="160"/>
+      <c r="AI534" s="160"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>